<commit_message>
`Refactor MainView, add database configuration and remove ReadExcel.py`
</commit_message>
<xml_diff>
--- a/app/utils/ComandosEletricos.xlsx
+++ b/app/utils/ComandosEletricos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Botao_comando" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="299">
   <si>
     <t>Formato</t>
   </si>
@@ -1271,7 +1271,7 @@
   <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,7 +1296,7 @@
       <c r="D1" t="s">
         <v>233</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3415,8 +3415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4790,7 +4790,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5221,7 +5221,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5520,8 +5520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5547,6 +5547,9 @@
       <c r="D1" t="s">
         <v>247</v>
       </c>
+      <c r="E1" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>